<commit_message>
Meta kaggle analysis for competitions
</commit_message>
<xml_diff>
--- a/meta-kaggle/kaggle-meta-schemas.xlsx
+++ b/meta-kaggle/kaggle-meta-schemas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rk/Desktop/data-analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rk/Desktop/data-analysis/meta-kaggle/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92186A0-058F-B746-B8C7-F32B1DEDE481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C934C2-4AE7-AD40-8A4C-F6FAFCE85D6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{AF090008-6B02-594E-B1D4-2E6B5F9F6F6D}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="223">
   <si>
     <t>Competitions.csv</t>
   </si>
@@ -690,13 +690,22 @@
     <t>Numeric</t>
   </si>
   <si>
-    <t>Null allowed?</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>Invalid data present - 0, Empty strings, Text</t>
+  </si>
+  <si>
+    <t>IntegerType</t>
+  </si>
+  <si>
+    <t>StringType</t>
+  </si>
+  <si>
+    <t>BooleanType</t>
   </si>
 </sst>
 </file>
@@ -734,7 +743,7 @@
       <name val="Droid Sans Mono"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -759,8 +768,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -768,33 +783,121 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFC14"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1106,13 +1209,14 @@
   <dimension ref="A1:R78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N81" sqref="N81"/>
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="46.83203125" style="2" customWidth="1"/>
-    <col min="2" max="3" width="26" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26" style="2" customWidth="1"/>
+    <col min="3" max="3" width="64.5" style="2" customWidth="1"/>
     <col min="4" max="4" width="2.83203125" style="2" customWidth="1"/>
     <col min="5" max="5" width="41.5" style="2" customWidth="1"/>
     <col min="6" max="6" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
@@ -1157,44 +1261,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="6" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="6"/>
+      <c r="F1" s="9"/>
       <c r="G1" s="4"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="6" t="s">
+      <c r="H1" s="6"/>
+      <c r="I1" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="J1" s="6"/>
+      <c r="J1" s="9"/>
       <c r="K1" s="4"/>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="N1" s="6"/>
+      <c r="N1" s="9"/>
       <c r="O1" s="4"/>
-      <c r="Q1" s="6" t="s">
+      <c r="Q1" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="R1" s="6"/>
+      <c r="R1" s="9"/>
     </row>
     <row r="2" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="7"/>
+      <c r="A2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="6"/>
       <c r="E2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="8"/>
+      <c r="H2" s="7"/>
       <c r="I2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1210,16 +1318,20 @@
       </c>
     </row>
     <row r="3" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="7"/>
+      <c r="B3" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="6"/>
       <c r="E3" s="3" t="s">
         <v>62</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
-      <c r="H3" s="8"/>
+      <c r="H3" s="7"/>
       <c r="I3" s="3" t="s">
         <v>62</v>
       </c>
@@ -1235,16 +1347,20 @@
       </c>
     </row>
     <row r="4" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="7"/>
+      <c r="B4" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="6"/>
       <c r="E4" s="3" t="s">
         <v>63</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="8"/>
+      <c r="H4" s="7"/>
       <c r="I4" s="3" t="s">
         <v>68</v>
       </c>
@@ -1260,16 +1376,20 @@
       </c>
     </row>
     <row r="5" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="7"/>
+      <c r="B5" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="C5" s="11"/>
+      <c r="D5" s="6"/>
       <c r="E5" s="3" t="s">
         <v>64</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="8"/>
+      <c r="H5" s="7"/>
       <c r="I5" s="3" t="s">
         <v>67</v>
       </c>
@@ -1285,16 +1405,20 @@
       </c>
     </row>
     <row r="6" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="7"/>
+      <c r="B6" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="6"/>
       <c r="E6" s="3" t="s">
         <v>65</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="8"/>
+      <c r="H6" s="7"/>
       <c r="I6" s="3" t="s">
         <v>66</v>
       </c>
@@ -1307,41 +1431,49 @@
       <c r="O6" s="3"/>
     </row>
     <row r="7" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="7"/>
+      <c r="B7" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="6"/>
       <c r="E7" s="3" t="s">
         <v>66</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="8"/>
+      <c r="H7" s="7"/>
       <c r="M7" s="3" t="s">
         <v>114</v>
       </c>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
-      <c r="Q7" s="6" t="s">
+      <c r="Q7" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="R7" s="6"/>
+      <c r="R7" s="9"/>
     </row>
     <row r="8" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="7"/>
+      <c r="B8" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="C8" s="11"/>
+      <c r="D8" s="6"/>
       <c r="E8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="6" t="s">
+      <c r="H8" s="7"/>
+      <c r="I8" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="J8" s="6"/>
+      <c r="J8" s="9"/>
       <c r="K8" s="4"/>
       <c r="M8" s="3" t="s">
         <v>115</v>
@@ -1353,16 +1485,20 @@
       </c>
     </row>
     <row r="9" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="7"/>
+      <c r="B9" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="C9" s="11"/>
+      <c r="D9" s="6"/>
       <c r="E9" s="3" t="s">
         <v>67</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
-      <c r="H9" s="8"/>
+      <c r="H9" s="7"/>
       <c r="I9" s="3" t="s">
         <v>1</v>
       </c>
@@ -1378,16 +1514,20 @@
       </c>
     </row>
     <row r="10" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="7"/>
+      <c r="B10" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="C10" s="11"/>
+      <c r="D10" s="6"/>
       <c r="E10" s="3" t="s">
         <v>68</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="8"/>
+      <c r="H10" s="7"/>
       <c r="I10" s="3" t="s">
         <v>97</v>
       </c>
@@ -1398,41 +1538,49 @@
       </c>
     </row>
     <row r="11" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="7"/>
+      <c r="B11" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="6"/>
       <c r="E11" s="3" t="s">
         <v>69</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
-      <c r="H11" s="8"/>
+      <c r="H11" s="7"/>
       <c r="I11" s="3" t="s">
         <v>98</v>
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
-      <c r="M11" s="6" t="s">
+      <c r="M11" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="N11" s="6"/>
+      <c r="N11" s="9"/>
       <c r="O11" s="4"/>
       <c r="Q11" s="5" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="7"/>
+      <c r="B12" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="6"/>
       <c r="E12" s="3" t="s">
         <v>70</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="8"/>
+      <c r="H12" s="7"/>
       <c r="I12" s="3" t="s">
         <v>99</v>
       </c>
@@ -1446,16 +1594,20 @@
       </c>
     </row>
     <row r="13" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="7"/>
+      <c r="B13" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="6"/>
       <c r="E13" s="3" t="s">
         <v>71</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
-      <c r="H13" s="8"/>
+      <c r="H13" s="7"/>
       <c r="I13" s="3" t="s">
         <v>100</v>
       </c>
@@ -1469,16 +1621,20 @@
       </c>
     </row>
     <row r="14" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="7"/>
+      <c r="B14" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="6"/>
       <c r="E14" s="3" t="s">
         <v>72</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
-      <c r="H14" s="8"/>
+      <c r="H14" s="7"/>
       <c r="I14" s="3" t="s">
         <v>101</v>
       </c>
@@ -1492,16 +1648,20 @@
       </c>
     </row>
     <row r="15" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="7"/>
+      <c r="B15" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="6"/>
       <c r="E15" s="3" t="s">
         <v>73</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
-      <c r="H15" s="8"/>
+      <c r="H15" s="7"/>
       <c r="I15" s="3" t="s">
         <v>102</v>
       </c>
@@ -1515,11 +1675,15 @@
       </c>
     </row>
     <row r="16" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="7"/>
-      <c r="H16" s="7"/>
+      <c r="B16" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="C16" s="11"/>
+      <c r="D16" s="6"/>
+      <c r="H16" s="6"/>
       <c r="I16" s="3" t="s">
         <v>103</v>
       </c>
@@ -1533,16 +1697,20 @@
       </c>
     </row>
     <row r="17" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="6" t="s">
+      <c r="B17" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="C17" s="11"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="F17" s="6"/>
+      <c r="F17" s="9"/>
       <c r="G17" s="4"/>
-      <c r="H17" s="7"/>
+      <c r="H17" s="6"/>
       <c r="I17" s="3" t="s">
         <v>104</v>
       </c>
@@ -1553,41 +1721,49 @@
       </c>
     </row>
     <row r="18" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="7"/>
+      <c r="B18" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="C18" s="11"/>
+      <c r="D18" s="6"/>
       <c r="E18" s="3" t="s">
         <v>1</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
-      <c r="H18" s="7"/>
+      <c r="H18" s="6"/>
       <c r="I18" s="3" t="s">
         <v>105</v>
       </c>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
-      <c r="M18" s="6" t="s">
+      <c r="M18" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="N18" s="6"/>
+      <c r="N18" s="9"/>
       <c r="O18" s="4"/>
       <c r="Q18" s="5" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="7"/>
+      <c r="B19" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="D19" s="6"/>
       <c r="E19" s="3" t="s">
         <v>75</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="7"/>
+      <c r="H19" s="6"/>
       <c r="M19" s="3" t="s">
         <v>1</v>
       </c>
@@ -1596,20 +1772,24 @@
       </c>
     </row>
     <row r="20" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="7"/>
+      <c r="B20" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="C20" s="11"/>
+      <c r="D20" s="6"/>
       <c r="E20" s="3" t="s">
         <v>44</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="6" t="s">
+      <c r="H20" s="6"/>
+      <c r="I20" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="J20" s="6"/>
+      <c r="J20" s="9"/>
       <c r="K20" s="4"/>
       <c r="M20" s="3" t="s">
         <v>122</v>
@@ -1619,11 +1799,15 @@
       </c>
     </row>
     <row r="21" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="7"/>
-      <c r="H21" s="7"/>
+      <c r="B21" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="C21" s="11"/>
+      <c r="D21" s="6"/>
+      <c r="H21" s="6"/>
       <c r="I21" s="3" t="s">
         <v>1</v>
       </c>
@@ -1637,16 +1821,20 @@
       </c>
     </row>
     <row r="22" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="7"/>
+      <c r="B22" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="C22" s="11"/>
+      <c r="D22" s="6"/>
       <c r="E22" s="4" t="s">
         <v>76</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
-      <c r="H22" s="7"/>
+      <c r="H22" s="6"/>
       <c r="I22" s="3" t="s">
         <v>67</v>
       </c>
@@ -1657,41 +1845,49 @@
       </c>
     </row>
     <row r="23" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="7"/>
+      <c r="B23" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="C23" s="11"/>
+      <c r="D23" s="6"/>
       <c r="E23" s="3" t="s">
         <v>1</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
-      <c r="H23" s="7"/>
+      <c r="H23" s="6"/>
       <c r="I23" s="3" t="s">
         <v>47</v>
       </c>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
-      <c r="M23" s="6" t="s">
+      <c r="M23" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="N23" s="6"/>
+      <c r="N23" s="9"/>
       <c r="O23" s="4"/>
       <c r="Q23" s="5" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="7"/>
+      <c r="B24" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="C24" s="11"/>
+      <c r="D24" s="6"/>
       <c r="E24" s="3" t="s">
         <v>75</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
-      <c r="H24" s="7"/>
+      <c r="H24" s="6"/>
       <c r="I24" s="3" t="s">
         <v>107</v>
       </c>
@@ -1702,16 +1898,20 @@
       </c>
     </row>
     <row r="25" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="7"/>
+      <c r="B25" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="C25" s="11"/>
+      <c r="D25" s="6"/>
       <c r="E25" s="3" t="s">
         <v>63</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
-      <c r="H25" s="7"/>
+      <c r="H25" s="6"/>
       <c r="I25" s="3" t="s">
         <v>108</v>
       </c>
@@ -1720,22 +1920,26 @@
       <c r="M25" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="Q25" s="6" t="s">
+      <c r="Q25" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="R25" s="6"/>
+      <c r="R25" s="9"/>
     </row>
     <row r="26" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D26" s="7"/>
+      <c r="B26" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="C26" s="11"/>
+      <c r="D26" s="6"/>
       <c r="E26" s="3" t="s">
         <v>68</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
-      <c r="H26" s="7"/>
+      <c r="H26" s="6"/>
       <c r="M26" s="3" t="s">
         <v>82</v>
       </c>
@@ -1744,20 +1948,24 @@
       </c>
     </row>
     <row r="27" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="D27" s="7"/>
+      <c r="B27" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="C27" s="11"/>
+      <c r="D27" s="6"/>
       <c r="E27" s="3" t="s">
         <v>77</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="6" t="s">
+      <c r="H27" s="6"/>
+      <c r="I27" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="J27" s="6"/>
+      <c r="J27" s="9"/>
       <c r="K27" s="4"/>
       <c r="M27" s="3" t="s">
         <v>124</v>
@@ -1767,16 +1975,20 @@
       </c>
     </row>
     <row r="28" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D28" s="7"/>
+      <c r="B28" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="C28" s="11"/>
+      <c r="D28" s="6"/>
       <c r="E28" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
-      <c r="H28" s="7"/>
+      <c r="H28" s="6"/>
       <c r="I28" s="5" t="s">
         <v>1</v>
       </c>
@@ -1788,16 +2000,20 @@
       </c>
     </row>
     <row r="29" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D29" s="7"/>
+      <c r="B29" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="C29" s="11"/>
+      <c r="D29" s="6"/>
       <c r="E29" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
-      <c r="H29" s="7"/>
+      <c r="H29" s="6"/>
       <c r="I29" s="5" t="s">
         <v>132</v>
       </c>
@@ -1806,38 +2022,46 @@
       </c>
     </row>
     <row r="30" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D30" s="7"/>
+      <c r="B30" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="C30" s="11"/>
+      <c r="D30" s="6"/>
       <c r="E30" s="3" t="s">
         <v>4</v>
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
-      <c r="H30" s="7"/>
+      <c r="H30" s="6"/>
       <c r="I30" s="5" t="s">
         <v>2</v>
       </c>
       <c r="M30" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="Q30" s="6" t="s">
+      <c r="Q30" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="R30" s="6"/>
+      <c r="R30" s="9"/>
     </row>
     <row r="31" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="D31" s="7"/>
+      <c r="B31" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="C31" s="11"/>
+      <c r="D31" s="6"/>
       <c r="E31" s="3" t="s">
         <v>78</v>
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
-      <c r="H31" s="7"/>
+      <c r="H31" s="6"/>
       <c r="I31" s="5" t="s">
         <v>68</v>
       </c>
@@ -1849,16 +2073,20 @@
       </c>
     </row>
     <row r="32" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="D32" s="7"/>
+      <c r="B32" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="C32" s="11"/>
+      <c r="D32" s="6"/>
       <c r="E32" s="3" t="s">
         <v>72</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
-      <c r="H32" s="7"/>
+      <c r="H32" s="6"/>
       <c r="I32" s="5" t="s">
         <v>77</v>
       </c>
@@ -1870,11 +2098,15 @@
       </c>
     </row>
     <row r="33" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="D33" s="7"/>
-      <c r="H33" s="7"/>
+      <c r="B33" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="C33" s="11"/>
+      <c r="D33" s="6"/>
+      <c r="H33" s="6"/>
       <c r="M33" s="3" t="s">
         <v>70</v>
       </c>
@@ -1883,58 +2115,70 @@
       </c>
     </row>
     <row r="34" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="D34" s="7"/>
+      <c r="B34" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="C34" s="11"/>
+      <c r="D34" s="6"/>
       <c r="E34" s="4" t="s">
         <v>79</v>
       </c>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="6" t="s">
+      <c r="H34" s="6"/>
+      <c r="I34" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="J34" s="6"/>
+      <c r="J34" s="9"/>
       <c r="K34" s="4"/>
       <c r="M34" s="3" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="35" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="D35" s="7"/>
+      <c r="B35" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="C35" s="11"/>
+      <c r="D35" s="6"/>
       <c r="E35" s="3" t="s">
         <v>1</v>
       </c>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
-      <c r="H35" s="7"/>
+      <c r="H35" s="6"/>
       <c r="I35" s="5" t="s">
         <v>1</v>
       </c>
       <c r="M35" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="Q35" s="6" t="s">
+      <c r="Q35" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="R35" s="6"/>
+      <c r="R35" s="9"/>
     </row>
     <row r="36" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="D36" s="7"/>
+      <c r="B36" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="C36" s="11"/>
+      <c r="D36" s="6"/>
       <c r="E36" s="3" t="s">
         <v>80</v>
       </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
-      <c r="H36" s="7"/>
+      <c r="H36" s="6"/>
       <c r="I36" s="5" t="s">
         <v>81</v>
       </c>
@@ -1946,16 +2190,20 @@
       </c>
     </row>
     <row r="37" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="D37" s="7"/>
+      <c r="B37" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="C37" s="11"/>
+      <c r="D37" s="6"/>
       <c r="E37" s="3" t="s">
         <v>81</v>
       </c>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
-      <c r="H37" s="7"/>
+      <c r="H37" s="6"/>
       <c r="I37" s="5" t="s">
         <v>169</v>
       </c>
@@ -1964,558 +2212,623 @@
       </c>
     </row>
     <row r="38" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="D38" s="7"/>
+      <c r="B38" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="C38" s="11"/>
+      <c r="D38" s="6"/>
       <c r="E38" s="3" t="s">
         <v>68</v>
       </c>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
-      <c r="H38" s="7"/>
+      <c r="H38" s="6"/>
       <c r="I38" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="M38" s="4" t="s">
+      <c r="M38" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="O38" s="2" t="s">
-        <v>217</v>
-      </c>
+      <c r="N38" s="15"/>
+      <c r="O38" s="16"/>
       <c r="Q38" s="5" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="39" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="D39" s="7"/>
+      <c r="B39" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="C39" s="11"/>
+      <c r="D39" s="6"/>
       <c r="E39" s="3" t="s">
         <v>82</v>
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
-      <c r="H39" s="7"/>
+      <c r="H39" s="6"/>
       <c r="I39" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="M39" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="N39" s="5" t="s">
+      <c r="M39" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="N39" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="O39" s="9" t="s">
-        <v>219</v>
+      <c r="O39" s="13" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="40" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="D40" s="7"/>
+      <c r="B40" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="C40" s="11"/>
+      <c r="D40" s="6"/>
       <c r="E40" s="3" t="s">
         <v>75</v>
       </c>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
-      <c r="H40" s="7"/>
+      <c r="H40" s="6"/>
       <c r="I40" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="M40" s="5" t="s">
+      <c r="M40" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="N40" s="5" t="s">
+      <c r="N40" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="O40" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="Q40" s="6" t="s">
+      <c r="O40" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="Q40" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="R40" s="6"/>
+      <c r="R40" s="9"/>
     </row>
     <row r="41" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="D41" s="7"/>
+      <c r="B41" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="C41" s="11"/>
+      <c r="D41" s="6"/>
       <c r="E41" s="3" t="s">
         <v>83</v>
       </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
-      <c r="H41" s="7"/>
+      <c r="H41" s="6"/>
       <c r="I41" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="M41" s="5" t="s">
+      <c r="M41" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="N41" s="5" t="s">
+      <c r="N41" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="O41" s="9" t="s">
-        <v>219</v>
+      <c r="O41" s="13" t="s">
+        <v>218</v>
       </c>
       <c r="Q41" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="D42" s="7"/>
-      <c r="H42" s="7"/>
+      <c r="B42" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="C42" s="11"/>
+      <c r="D42" s="6"/>
+      <c r="H42" s="6"/>
       <c r="I42" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="M42" s="5" t="s">
+      <c r="M42" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="N42" s="5" t="s">
+      <c r="N42" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="O42" s="9" t="s">
-        <v>219</v>
+      <c r="O42" s="13" t="s">
+        <v>218</v>
       </c>
       <c r="Q42" s="5" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="43" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="D43" s="7"/>
+      <c r="B43" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="C43" s="11"/>
+      <c r="D43" s="6"/>
       <c r="E43" s="4" t="s">
         <v>84</v>
       </c>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
-      <c r="H43" s="7"/>
+      <c r="H43" s="6"/>
       <c r="I43" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="M43" s="5" t="s">
+      <c r="M43" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="N43" s="5" t="s">
+      <c r="N43" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="O43" s="9" t="s">
-        <v>218</v>
+      <c r="O43" s="13" t="s">
+        <v>217</v>
       </c>
       <c r="Q43" s="5" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="44" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="D44" s="7"/>
+      <c r="D44" s="6"/>
       <c r="E44" s="3" t="s">
         <v>1</v>
       </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
-      <c r="H44" s="7"/>
+      <c r="H44" s="6"/>
       <c r="I44" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="M44" s="5" t="s">
+      <c r="M44" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="N44" s="5" t="s">
+      <c r="N44" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="O44" s="9" t="s">
-        <v>219</v>
+      <c r="O44" s="13" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="45" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A45" s="6" t="s">
+      <c r="A45" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B45" s="6"/>
+      <c r="B45" s="9"/>
       <c r="C45" s="4"/>
-      <c r="D45" s="7"/>
+      <c r="D45" s="6"/>
       <c r="E45" s="3" t="s">
         <v>75</v>
       </c>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
-      <c r="H45" s="7"/>
+      <c r="H45" s="6"/>
       <c r="I45" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="M45" s="5" t="s">
+      <c r="M45" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="N45" s="5" t="s">
+      <c r="N45" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="O45" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="Q45" s="6" t="s">
+      <c r="O45" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q45" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="R45" s="6"/>
+      <c r="R45" s="9"/>
     </row>
     <row r="46" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A46" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="7"/>
+      <c r="A46" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46" s="19"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="6"/>
       <c r="E46" s="3" t="s">
         <v>85</v>
       </c>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
-      <c r="H46" s="7"/>
-      <c r="M46" s="5" t="s">
+      <c r="H46" s="6"/>
+      <c r="M46" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="N46" s="5" t="s">
+      <c r="N46" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="O46" s="9" t="s">
-        <v>218</v>
+      <c r="O46" s="13" t="s">
+        <v>217</v>
       </c>
       <c r="Q46" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="7"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="6"/>
       <c r="E47" s="3" t="s">
         <v>62</v>
       </c>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
-      <c r="H47" s="7"/>
-      <c r="I47" s="4" t="s">
+      <c r="H47" s="6"/>
+      <c r="I47" s="12" t="s">
         <v>177</v>
       </c>
-      <c r="M47" s="5" t="s">
+      <c r="J47" s="12"/>
+      <c r="K47" s="12"/>
+      <c r="M47" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="N47" s="5" t="s">
+      <c r="N47" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="O47" s="9" t="s">
-        <v>219</v>
+      <c r="O47" s="13" t="s">
+        <v>218</v>
       </c>
       <c r="Q47" s="5" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="48" spans="1:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="A48" s="3" t="s">
+      <c r="A48" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="7"/>
+      <c r="B48" s="19"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="6"/>
       <c r="E48" s="3" t="s">
         <v>86</v>
       </c>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
-      <c r="H48" s="7"/>
-      <c r="I48" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="M48" s="5" t="s">
+      <c r="H48" s="6"/>
+      <c r="I48" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="J48" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="K48" s="11"/>
+      <c r="M48" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="N48" s="5" t="s">
+      <c r="N48" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="O48" s="9" t="s">
-        <v>219</v>
+      <c r="O48" s="13" t="s">
+        <v>218</v>
       </c>
       <c r="Q48" s="5" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="49" spans="4:17" ht="21" x14ac:dyDescent="0.3">
-      <c r="D49" s="7"/>
+      <c r="D49" s="6"/>
       <c r="E49" s="3" t="s">
         <v>68</v>
       </c>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
-      <c r="H49" s="7"/>
-      <c r="I49" s="5" t="s">
+      <c r="H49" s="6"/>
+      <c r="I49" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="M49" s="5" t="s">
+      <c r="J49" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="K49" s="11"/>
+      <c r="M49" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="N49" s="5" t="s">
+      <c r="N49" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="O49" s="9" t="s">
-        <v>219</v>
+      <c r="O49" s="13" t="s">
+        <v>218</v>
       </c>
       <c r="Q49" s="5" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="50" spans="4:17" ht="21" x14ac:dyDescent="0.3">
-      <c r="D50" s="7"/>
+      <c r="D50" s="6"/>
       <c r="E50" s="3" t="s">
         <v>87</v>
       </c>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
-      <c r="H50" s="7"/>
-      <c r="I50" s="5" t="s">
+      <c r="H50" s="6"/>
+      <c r="I50" s="10" t="s">
         <v>132</v>
       </c>
+      <c r="J50" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="K50" s="11"/>
       <c r="Q50" s="5" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="51" spans="4:17" ht="21" x14ac:dyDescent="0.3">
-      <c r="D51" s="7"/>
+      <c r="D51" s="6"/>
       <c r="E51" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
-      <c r="H51" s="7"/>
-      <c r="I51" s="5" t="s">
+      <c r="H51" s="6"/>
+      <c r="I51" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="M51" s="4" t="s">
+      <c r="J51" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="K51" s="11"/>
+      <c r="M51" s="9" t="s">
         <v>206</v>
       </c>
+      <c r="N51" s="9"/>
+      <c r="O51" s="9"/>
       <c r="Q51" s="5" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="52" spans="4:17" ht="21" x14ac:dyDescent="0.3">
-      <c r="D52" s="7"/>
+      <c r="D52" s="6"/>
       <c r="E52" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
-      <c r="H52" s="7"/>
-      <c r="I52" s="5" t="s">
+      <c r="H52" s="6"/>
+      <c r="I52" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="M52" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="N52" s="5" t="s">
+      <c r="J52" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="K52" s="11"/>
+      <c r="M52" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="N52" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="O52" s="5"/>
+      <c r="O52" s="10"/>
       <c r="Q52" s="5" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="53" spans="4:17" ht="21" x14ac:dyDescent="0.3">
-      <c r="D53" s="7"/>
+      <c r="D53" s="6"/>
       <c r="E53" s="3" t="s">
         <v>4</v>
       </c>
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
-      <c r="H53" s="7"/>
-      <c r="I53" s="5" t="s">
+      <c r="H53" s="6"/>
+      <c r="I53" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="M53" s="5" t="s">
+      <c r="J53" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="K53" s="11"/>
+      <c r="M53" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="N53" s="5" t="s">
+      <c r="N53" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="O53" s="5"/>
+      <c r="O53" s="10"/>
       <c r="Q53" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="54" spans="4:17" ht="21" x14ac:dyDescent="0.3">
-      <c r="D54" s="7"/>
+      <c r="D54" s="6"/>
       <c r="E54" s="3" t="s">
         <v>77</v>
       </c>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
-      <c r="H54" s="7"/>
-      <c r="I54" s="5" t="s">
+      <c r="H54" s="6"/>
+      <c r="I54" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="M54" s="5" t="s">
+      <c r="J54" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="K54" s="11"/>
+      <c r="M54" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="N54" s="5" t="s">
+      <c r="N54" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="O54" s="5"/>
+      <c r="O54" s="10"/>
       <c r="Q54" s="5" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="55" spans="4:17" ht="21" x14ac:dyDescent="0.3">
-      <c r="D55" s="7"/>
+      <c r="D55" s="6"/>
       <c r="E55" s="3" t="s">
         <v>88</v>
       </c>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
-      <c r="H55" s="7"/>
-      <c r="I55" s="5" t="s">
+      <c r="H55" s="6"/>
+      <c r="I55" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="M55" s="5" t="s">
+      <c r="J55" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="K55" s="11"/>
+      <c r="M55" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="N55" s="5" t="s">
+      <c r="N55" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="O55" s="5"/>
+      <c r="O55" s="10"/>
       <c r="Q55" s="5" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="56" spans="4:17" ht="21" x14ac:dyDescent="0.3">
-      <c r="D56" s="7"/>
+      <c r="D56" s="6"/>
       <c r="E56" s="3" t="s">
         <v>89</v>
       </c>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
-      <c r="H56" s="7"/>
-      <c r="I56" s="5" t="s">
+      <c r="H56" s="6"/>
+      <c r="I56" s="10" t="s">
         <v>182</v>
       </c>
+      <c r="J56" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="K56" s="11"/>
       <c r="Q56" s="5" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="57" spans="4:17" ht="21" x14ac:dyDescent="0.3">
-      <c r="D57" s="7"/>
+      <c r="D57" s="6"/>
       <c r="E57" s="3" t="s">
         <v>90</v>
       </c>
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
-      <c r="H57" s="7"/>
-      <c r="M57" s="4" t="s">
+      <c r="H57" s="6"/>
+      <c r="M57" s="9" t="s">
         <v>208</v>
       </c>
+      <c r="N57" s="9"/>
+      <c r="O57" s="9"/>
       <c r="Q57" s="5" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="58" spans="4:17" ht="21" x14ac:dyDescent="0.3">
-      <c r="D58" s="7"/>
-      <c r="H58" s="7"/>
+      <c r="D58" s="6"/>
+      <c r="H58" s="6"/>
       <c r="I58" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="M58" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="N58" s="5" t="s">
+      <c r="M58" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="N58" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="O58" s="5"/>
+      <c r="O58" s="10"/>
       <c r="Q58" s="5" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="59" spans="4:17" ht="21" x14ac:dyDescent="0.3">
-      <c r="D59" s="7"/>
+      <c r="D59" s="6"/>
       <c r="E59" s="4" t="s">
         <v>91</v>
       </c>
       <c r="F59" s="4"/>
       <c r="G59" s="4"/>
-      <c r="H59" s="7"/>
+      <c r="H59" s="6"/>
       <c r="I59" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="M59" s="5" t="s">
+      <c r="M59" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="N59" s="5" t="s">
+      <c r="N59" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="O59" s="5"/>
+      <c r="O59" s="10"/>
       <c r="Q59" s="5" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="60" spans="4:17" ht="21" x14ac:dyDescent="0.3">
-      <c r="D60" s="7"/>
+      <c r="D60" s="6"/>
       <c r="E60" s="3" t="s">
         <v>1</v>
       </c>
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
-      <c r="H60" s="7"/>
+      <c r="H60" s="6"/>
       <c r="I60" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="M60" s="5" t="s">
+      <c r="M60" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="N60" s="5" t="s">
+      <c r="N60" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="O60" s="5"/>
+      <c r="O60" s="10"/>
       <c r="Q60" s="5" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="61" spans="4:17" ht="21" x14ac:dyDescent="0.3">
-      <c r="D61" s="7"/>
+      <c r="D61" s="6"/>
       <c r="E61" s="3" t="s">
         <v>92</v>
       </c>
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
-      <c r="H61" s="7"/>
+      <c r="H61" s="6"/>
       <c r="I61" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="M61" s="5" t="s">
+      <c r="M61" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="N61" s="5" t="s">
+      <c r="N61" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="O61" s="5"/>
+      <c r="O61" s="10"/>
       <c r="Q61" s="5" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="62" spans="4:17" ht="21" x14ac:dyDescent="0.3">
-      <c r="D62" s="7"/>
+      <c r="D62" s="6"/>
       <c r="E62" s="3" t="s">
         <v>93</v>
       </c>
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
-      <c r="H62" s="7"/>
+      <c r="H62" s="6"/>
       <c r="I62" s="5" t="s">
         <v>184</v>
       </c>
@@ -2524,264 +2837,273 @@
       </c>
     </row>
     <row r="63" spans="4:17" ht="21" x14ac:dyDescent="0.3">
-      <c r="D63" s="7"/>
+      <c r="D63" s="6"/>
       <c r="E63" s="3" t="s">
         <v>94</v>
       </c>
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
-      <c r="H63" s="7"/>
-      <c r="M63" s="4" t="s">
+      <c r="H63" s="6"/>
+      <c r="M63" s="14" t="s">
         <v>210</v>
       </c>
+      <c r="N63" s="15"/>
+      <c r="O63" s="16"/>
       <c r="Q63" s="5" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="64" spans="4:17" ht="21" x14ac:dyDescent="0.3">
-      <c r="D64" s="7"/>
-      <c r="H64" s="7"/>
+      <c r="D64" s="6"/>
+      <c r="H64" s="6"/>
       <c r="I64" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="M64" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="N64" s="5" t="s">
+      <c r="M64" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="N64" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="O64" s="5"/>
+      <c r="O64" s="10"/>
       <c r="Q64" s="5" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="65" spans="4:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="D65" s="7"/>
-      <c r="H65" s="7"/>
+      <c r="D65" s="6"/>
+      <c r="H65" s="6"/>
       <c r="I65" s="5" t="s">
         <v>1</v>
       </c>
       <c r="J65" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="K65" s="9"/>
-      <c r="M65" s="5" t="s">
+      <c r="K65" s="8"/>
+      <c r="M65" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="N65" s="5" t="s">
+      <c r="N65" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="O65" s="5"/>
+      <c r="O65" s="10"/>
     </row>
     <row r="66" spans="4:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="D66" s="7"/>
-      <c r="H66" s="7"/>
+      <c r="D66" s="6"/>
+      <c r="H66" s="6"/>
       <c r="I66" s="5" t="s">
         <v>47</v>
       </c>
       <c r="J66" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="K66" s="9"/>
-      <c r="M66" s="5" t="s">
+      <c r="K66" s="8"/>
+      <c r="M66" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="N66" s="5" t="s">
+      <c r="N66" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="O66" s="5"/>
-      <c r="Q66" s="6" t="s">
+      <c r="O66" s="10"/>
+      <c r="Q66" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="R66" s="6"/>
-    </row>
-    <row r="67" spans="4:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="D67" s="7"/>
-      <c r="H67" s="7"/>
+      <c r="R66" s="9"/>
+    </row>
+    <row r="67" spans="4:18" ht="44" x14ac:dyDescent="0.3">
+      <c r="D67" s="6"/>
+      <c r="H67" s="6"/>
       <c r="I67" s="5" t="s">
         <v>186</v>
       </c>
       <c r="J67" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="K67" s="9"/>
-      <c r="M67" s="5" t="s">
+      <c r="K67" s="8"/>
+      <c r="M67" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="N67" s="5" t="s">
+      <c r="N67" s="17" t="s">
         <v>215</v>
       </c>
-      <c r="O67" s="5"/>
+      <c r="O67" s="18" t="s">
+        <v>219</v>
+      </c>
       <c r="Q67" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="68" spans="4:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="D68" s="7"/>
-      <c r="H68" s="7"/>
+      <c r="D68" s="6"/>
+      <c r="H68" s="6"/>
       <c r="I68" s="5" t="s">
         <v>187</v>
       </c>
       <c r="J68" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="K68" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="M68" s="5" t="s">
+      <c r="K68" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="M68" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="N68" s="5" t="s">
+      <c r="N68" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="O68" s="5"/>
+      <c r="O68" s="10"/>
       <c r="Q68" s="5" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="69" spans="4:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="D69" s="7"/>
-      <c r="H69" s="7"/>
+      <c r="D69" s="6"/>
+      <c r="H69" s="6"/>
       <c r="I69" s="5" t="s">
         <v>188</v>
       </c>
       <c r="J69" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="K69" s="9" t="s">
-        <v>218</v>
+      <c r="K69" s="8" t="s">
+        <v>217</v>
       </c>
       <c r="Q69" s="5" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="70" spans="4:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="D70" s="7"/>
-      <c r="H70" s="7"/>
+      <c r="D70" s="6"/>
+      <c r="H70" s="6"/>
       <c r="I70" s="5" t="s">
         <v>189</v>
       </c>
       <c r="J70" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="K70" s="9" t="s">
-        <v>218</v>
+      <c r="K70" s="8" t="s">
+        <v>217</v>
       </c>
       <c r="Q70" s="5" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="71" spans="4:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="D71" s="7"/>
-      <c r="H71" s="7"/>
+      <c r="D71" s="6"/>
+      <c r="H71" s="6"/>
       <c r="I71" s="5" t="s">
         <v>190</v>
       </c>
       <c r="J71" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="K71" s="9" t="s">
-        <v>218</v>
+      <c r="K71" s="8" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="72" spans="4:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="D72" s="7"/>
-      <c r="H72" s="7"/>
+      <c r="D72" s="6"/>
+      <c r="H72" s="6"/>
       <c r="I72" s="5" t="s">
         <v>191</v>
       </c>
       <c r="J72" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="K72" s="9" t="s">
-        <v>218</v>
+      <c r="K72" s="8" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="73" spans="4:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="D73" s="7"/>
-      <c r="H73" s="7"/>
+      <c r="D73" s="6"/>
+      <c r="H73" s="6"/>
       <c r="I73" s="5" t="s">
         <v>192</v>
       </c>
       <c r="J73" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="K73" s="9"/>
+      <c r="K73" s="8"/>
     </row>
     <row r="74" spans="4:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="D74" s="7"/>
-      <c r="H74" s="7"/>
+      <c r="D74" s="6"/>
+      <c r="H74" s="6"/>
       <c r="I74" s="5" t="s">
         <v>115</v>
       </c>
       <c r="J74" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="K74" s="9" t="s">
-        <v>218</v>
+      <c r="K74" s="8" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="75" spans="4:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="D75" s="7"/>
-      <c r="H75" s="7"/>
+      <c r="D75" s="6"/>
+      <c r="H75" s="6"/>
       <c r="I75" s="5" t="s">
         <v>116</v>
       </c>
       <c r="J75" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="K75" s="9"/>
+      <c r="K75" s="8"/>
     </row>
     <row r="76" spans="4:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="D76" s="7"/>
-      <c r="H76" s="7"/>
+      <c r="D76" s="6"/>
+      <c r="H76" s="6"/>
       <c r="I76" s="5" t="s">
         <v>193</v>
       </c>
       <c r="J76" s="5"/>
-      <c r="K76" s="9"/>
+      <c r="K76" s="8"/>
     </row>
     <row r="77" spans="4:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="D77" s="7"/>
-      <c r="H77" s="7"/>
+      <c r="D77" s="6"/>
+      <c r="H77" s="6"/>
       <c r="I77" s="5" t="s">
         <v>194</v>
       </c>
       <c r="J77" s="5"/>
-      <c r="K77" s="9"/>
+      <c r="K77" s="8"/>
     </row>
     <row r="78" spans="4:18" ht="21" x14ac:dyDescent="0.3">
-      <c r="D78" s="7"/>
-      <c r="H78" s="7"/>
+      <c r="D78" s="6"/>
+      <c r="H78" s="6"/>
       <c r="I78" s="5" t="s">
         <v>195</v>
       </c>
       <c r="J78" s="5"/>
-      <c r="K78" s="9"/>
+      <c r="K78" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="Q40:R40"/>
-    <mergeCell ref="Q45:R45"/>
-    <mergeCell ref="Q66:R66"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="Q25:R25"/>
-    <mergeCell ref="Q30:R30"/>
-    <mergeCell ref="Q35:R35"/>
+  <mergeCells count="26">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="I47:K47"/>
+    <mergeCell ref="A1:C1"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="I8:J8"/>
     <mergeCell ref="I20:J20"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="M11:N11"/>
     <mergeCell ref="M18:N18"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="Q30:R30"/>
+    <mergeCell ref="Q40:R40"/>
+    <mergeCell ref="Q45:R45"/>
+    <mergeCell ref="Q66:R66"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="Q35:R35"/>
+    <mergeCell ref="M63:O63"/>
+    <mergeCell ref="M38:O38"/>
+    <mergeCell ref="M51:O51"/>
+    <mergeCell ref="M57:O57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>